<commit_message>
Alguns conflitos na aula 6
</commit_message>
<xml_diff>
--- a/SENAI-Sprint.1-BD/1.1/Modelo-Fisico.xlsx
+++ b/SENAI-Sprint.1-BD/1.1/Modelo-Fisico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flávia\Documents\Técnico\Segundo semestre\SENAI-Segundo.Semestre\SENAI-Sprint.1-BD\1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flávia\Documents\Python Scripts\Técnico\Segundo semestre\SENAI-Segundo.Semestre\SENAI-Sprint.1-BD\1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E7B65B-E393-4711-88F4-CF158FA36E5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AF1E34-F8C4-43E6-9C07-F266D698AE1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00267F44-AF11-48F9-B871-E9C2996A54E6}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00267F44-AF11-48F9-B871-E9C2996A54E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercicio 1.1" sheetId="2" r:id="rId1"/>
@@ -555,7 +555,7 @@
   <dimension ref="B2:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +608,7 @@
         <v>14</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>